<commit_message>
Ground alt was corrected
</commit_message>
<xml_diff>
--- a/MATLAB/Simulation/Data.xlsx
+++ b/MATLAB/Simulation/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4B1BFE-7FF0-4EAE-8AA6-FC9861C205FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934EA4D9-4E96-4AF1-98BF-65ABBF28749F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27810" windowHeight="15480" tabRatio="725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -729,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,7 +1095,7 @@
         <v>47</v>
       </c>
       <c r="B26" s="1">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>

</xml_diff>